<commit_message>
Test cases for a PRECINCT01
</commit_message>
<xml_diff>
--- a/InputFiles/ICDC/TC011_Canine_Filter_Study-PRECINCT01.xlsx
+++ b/InputFiles/ICDC/TC011_Canine_Filter_Study-PRECINCT01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\JanBranch\Commons_Automation\InputFiles\ICDC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\epishinavv\git\Commons_Automation\InputFiles\ICDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F56BEA5-49DB-4783-A3B5-1FCB288DF7CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5374BF4B-A1C3-48B6-B543-307F49C1CC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="35520" yWindow="5865" windowWidth="18780" windowHeight="10200" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -66,6 +66,38 @@
     <t>TC011_Canine_Filter_Study-PRECINCT01_WebData.xlsx</t>
   </si>
   <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
+WHERE s.clinical_study_designation IN ['PRECINCT01'] WITH DISTINCT samp AS samp, c, demo, diag
+RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
+        coalesce(c.case_id, '') AS `Case ID`, 
+        coalesce(demo.breed,'') AS Breed , 
+        coalesce(diag.disease_term,'') AS Diagnosis , 
+        coalesce(samp.sample_site, '') AS `Sample Site`,
+        coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
+        coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
+        coalesce(samp.tumor_grade, '') AS `Tumor Grade`,
+        coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
+        coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
+        coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
+        coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
+  </si>
+  <si>
+    <t>MATCH (p:program)&lt;--(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (diag:diagnosis)--&gt;(c)
+OPTIONAL MATCH (f:file)-[*]-&gt;(c)
+OPTIONAL MATCH (sf:file)--&gt;(s)
+WITH DISTINCT f, sf, samp AS samp, c, demo, diag, s, p
+WHERE s.clinical_study_designation IN ['PRECINCT01']
+RETURN  
+    count(distinct p) AS Programs,
+    count(distinct s) AS Studies,
+    count(distinct c) AS Cases,
+    count(distinct samp) AS Samples,
+    count(distinct f) AS `Case Files`,
+    count(distinct sf) AS `Study Files`</t>
+  </si>
+  <si>
     <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
 WHERE s.clinical_study_designation IN ['PRECINCT01'] 
 MATCH (c)&lt;--(diag:diagnosis)
@@ -83,46 +115,15 @@
         coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
         coalesce(demo.weight, '') AS `Weight (kg)`,
         coalesce(diag.best_response, '') AS `Response to Treatment`,
-        coalesce(co.cohort_description, '') AS `Cohort`</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
-WHERE s.clinical_study_designation IN ['PRECINCT01'] WITH DISTINCT samp AS samp, c, demo, diag
-RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
-        coalesce(c.case_id, '') AS `Case ID`, 
-        coalesce(demo.breed,'') AS Breed , 
-        coalesce(diag.disease_term,'') AS Diagnosis , 
-        coalesce(samp.sample_site, '') AS `Sample Site`,
-        coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
-        coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
-        coalesce(samp.tumor_grade, '') AS `Tumor Grade`,
-        coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
-        coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
-        coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
-        coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
-  </si>
-  <si>
-    <t>MATCH (f:file)--&gt;(parent)
-WITH DISTINCT f, parent
-MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
- MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
-WHERE s.clinical_study_designation IN ['PRECINCT01'] 
-WITH DISTINCT f, parent, c, demo, diag, s
-RETURN coalesce(f.file_name, '') AS `File Name`, 
-        coalesce(labels(parent)[0], '') AS `Association`,
-        coalesce(f.file_description, '') AS `Description`,
-        coalesce(f.file_format, '') AS `Format`,
-        coalesce(f.file_size, '') AS `Size`,
-        coalesce(c.case_id, '') AS `Case ID`, 
-        coalesce(diag.disease_term,'') AS Diagnosis , 
-        coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
+        coalesce(co.cohort_description, '') AS `Cohort`
+        order by c.case_id asc
+limit 100</t>
   </si>
   <si>
     <t>MATCH (f:file)--&gt;(s:study)
+WHERE s.clinical_study_designation IN ['PRECINCT01']
 MATCH (s)&lt;--(c:case)&lt;--(diag:diagnosis)
 MATCH (c)&lt;--(demo:demographic)
-MATCH (samp:sample)--&gt;(c)
-WHERE s.clinical_study_designation IN ['PRECINCT01'] and diag.best_response in ['Not Applicable']
 WITH
         DISTINCT f, c, demo, diag, s,
         ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
@@ -147,20 +148,37 @@
   limit 100</t>
   </si>
   <si>
-    <t>MATCH (p:program)&lt;--(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
-OPTIONAL MATCH (samp:sample)--&gt;(c)
-OPTIONAL MATCH (diag:diagnosis)--&gt;(c)
-OPTIONAL MATCH (f:file)-[*]-&gt;(c)
-OPTIONAL MATCH (sf:file)--&gt;(s)
-WITH DISTINCT f, sf, samp AS samp, c, demo, diag, s, p
+    <t>MATCH (f:file)--&gt;(parent)
+MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
+MATCH (diag:diagnosis)--&gt;(c)
+MATCH (s:study)&lt;--(c)
 WHERE s.clinical_study_designation IN ['PRECINCT01']
-RETURN  
-    count(distinct p) AS Programs,
-    count(distinct s) AS Studies,
-    count(distinct c) AS Cases,
-    count(distinct samp) AS Samples,
-    count(distinct f) AS `Case Files`,
-    count(distinct sf) AS `Study Files`</t>
+OPTIONAL MATCH (f)-[*]-&gt;(samp:sample)
+WITH
+        DISTINCT f, parent, c, demo, diag, s, samp,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(f.file_size)/log(1024))) as i,
+        2 as precision
+WITH
+        f, parent, c, demo, diag, s, samp,
+        f.file_size /(1024^i) AS value,
+        10^precision AS factor,
+        units[i] as unit
+WITH
+        f, parent, c, demo, diag, s, samp, unit,
+        round(factor * value)/factor AS size
+RETURN
+        coalesce(f.file_name, '') AS `File Name`,
+        coalesce(f.file_format, '') AS `Format`,
+        coalesce(f.file_type, '') AS `File Type`,
+        CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
+        coalesce(labels(parent)[0], '') AS `Association`,
+        coalesce(f.file_description, '') AS `Description`,
+        coalesce(samp.sample_id, '') AS `Sample ID`,
+        coalesce(c.case_id, '') AS `Case ID`,
+        coalesce(demo.breed,'') AS Breed ,
+        coalesce(diag.disease_term,'') AS Diagnosis
+        order by f.file_name asc limit 100</t>
   </si>
 </sst>
 </file>
@@ -245,9 +263,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -285,7 +303,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -391,7 +409,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -533,7 +551,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -543,19 +561,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="75.85546875" customWidth="1"/>
-    <col min="4" max="4" width="70.28515625" customWidth="1"/>
-    <col min="5" max="5" width="51.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="75.81640625" customWidth="1"/>
+    <col min="4" max="4" width="70.26953125" customWidth="1"/>
+    <col min="5" max="5" width="51.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -572,15 +590,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="270" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="290" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -589,15 +607,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="240" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -606,15 +624,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -623,7 +641,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -631,7 +649,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>

</xml_diff>